<commit_message>
Added arguments to APL/CMACGM/Evergreen/OOCL to take the write path from the threading config file
</commit_message>
<xml_diff>
--- a/APL/Test.xlsx
+++ b/APL/Test.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvanausdeln\Dropbox (Blume Global)\Documents\UiPath\RPA-Data-Scraping\ShippingStatusTool\APL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\blume-proj\OceanCarrierRPA\APL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17730"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Container" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -546,7 +546,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F21"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>